<commit_message>
update function: edit product info
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -1,34 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eang hengty\Documents\Small Python Project 2025\Simple Inventory Tracker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B46E48-B7E5-4B85-B32F-DECA0121FB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Logs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Last Updated</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Iphone 8</t>
+  </si>
+  <si>
+    <t>pcs</t>
+  </si>
+  <si>
+    <t>2025-04-19</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>iphone 7</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>New Stock</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Stock In</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +108,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,99 +410,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Product ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Product Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Stock</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Unit</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Last Updated</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>iphone 5</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>pcs</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2025-04-19</t>
-        </is>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>iphone 7</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>pcs</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2025-04-19</t>
-        </is>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update minor change on fucntion update product
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -1,95 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eang hengty\Documents\Small Python Project 2025\Simple Inventory Tracker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B46E48-B7E5-4B85-B32F-DECA0121FB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Logs" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Logs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
-  <si>
-    <t>Product ID</t>
-  </si>
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>Stock</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Last Updated</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Iphone 8</t>
-  </si>
-  <si>
-    <t>pcs</t>
-  </si>
-  <si>
-    <t>2025-04-19</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>iphone 7</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Change</t>
-  </si>
-  <si>
-    <t>New Stock</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Stock In</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,21 +48,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -410,70 +409,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Product ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Product Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Stock</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Last Updated</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Iphone5</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2025-04-19</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Iphone8</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-04-19</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -482,45 +520,113 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Product ID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>New Stock</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Action</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-04-19</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>-5</v>
+      </c>
+      <c r="D2" t="n">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Stock Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-04-19</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Stock Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-04-19</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Stock Out</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new function delete product
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,16 +457,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Iphone5</t>
+          <t>Iphone8</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -479,36 +479,6 @@
         </is>
       </c>
       <c r="F2" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Iphone8</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>pcs</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2025-04-19</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
@@ -525,7 +495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,6 +599,33 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Deleted</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
[minor update - add name who delete] to delete product function
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -2,16 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Logs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -51,7 +50,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -414,13 +413,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -481,6 +480,36 @@
       <c r="F2" t="inlineStr">
         <is>
           <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>IphoneX</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -495,13 +524,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="10.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -623,6 +655,107 @@
       <c r="E5" t="inlineStr">
         <is>
           <t>Deleted</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>-6</v>
+      </c>
+      <c r="D6" t="n">
+        <v>9</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Stock Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>-6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Stock Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>-5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Stock Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Deleted</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Hengty</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
[new feature - search product by name or id] added to the SIV
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Logs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +51,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -415,11 +416,11 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -456,16 +457,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Iphone8</t>
+          <t>doll</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -474,7 +475,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-04-19</t>
+          <t>2025-04-20</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -486,16 +487,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>IphoneX</t>
+          <t>Pen toy</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -509,7 +510,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>LOW</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -524,16 +525,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="10.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -565,7 +563,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-04-19</t>
+          <t>2025-04-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -584,178 +582,9 @@
           <t>Stock Out</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2025-04-19</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Stock Out</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2025-04-19</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Stock Out</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2025-04-20</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Deleted</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2025-04-20</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>-6</v>
-      </c>
-      <c r="D6" t="n">
-        <v>9</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Stock Out</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2025-04-20</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>-6</v>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Stock Out</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2025-04-20</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>-5</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Stock Out</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-04-20</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Deleted</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Hengty</t>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>hengty</t>
         </is>
       </c>
     </row>

</xml_diff>